<commit_message>
Updated dGLN3 gene list
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/GRN_Gene_Lists.xlsx
+++ b/data/GRNmap_input_workbooks/GRN_Gene_Lists.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13960" tabRatio="500"/>
+    <workbookView xWindow="11200" yWindow="1820" windowWidth="25600" windowHeight="13960" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="wt_gene_list" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -121,6 +121,22 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,8 +168,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -162,7 +190,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -506,82 +546,77 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>25</v>
+      <c r="A6" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>4</v>
+      <c r="A7" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>5</v>
+      <c r="A8" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>6</v>
+      <c r="A9" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>7</v>
+      <c r="A10" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>8</v>
+      <c r="A11" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>9</v>
+      <c r="A12" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>10</v>
+      <c r="A13" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>11</v>
+      <c r="A14" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>12</v>
+      <c r="A15" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -697,10 +732,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -752,31 +787,37 @@
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -790,7 +831,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -877,6 +918,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -977,6 +1019,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add sheet for gene lists for all strains
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/GRN_Gene_Lists.xlsx
+++ b/data/GRNmap_input_workbooks/GRN_Gene_Lists.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdahlqui\Documents\GitClone_DahlquistLab_20160622b\DahlquistLab\data\GRNmap_input_workbooks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="1820" windowWidth="25600" windowHeight="13960" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="11205" yWindow="1815" windowWidth="25605" windowHeight="13965" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="wt_gene_list" sheetId="1" r:id="rId1"/>
@@ -12,6 +17,7 @@
     <sheet name="dGLN3_gene_list" sheetId="3" r:id="rId3"/>
     <sheet name="dHAP4_gene_list" sheetId="4" r:id="rId4"/>
     <sheet name="dZAP1_gene_list" sheetId="5" r:id="rId5"/>
+    <sheet name="all-strains_gene_list" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="32">
   <si>
     <t>ABF1</t>
   </si>
@@ -104,13 +110,28 @@
   </si>
   <si>
     <t>CST6</t>
+  </si>
+  <si>
+    <t>wt_list</t>
+  </si>
+  <si>
+    <t>dCIN5_list</t>
+  </si>
+  <si>
+    <t>dGLN3_list</t>
+  </si>
+  <si>
+    <t>dHAP4_list</t>
+  </si>
+  <si>
+    <t>dZAP1_list</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,13 +162,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -183,12 +236,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -207,6 +269,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -535,87 +605,87 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -638,84 +708,84 @@
       <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -734,83 +804,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -834,84 +904,84 @@
       <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -935,84 +1005,84 @@
       <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1026,4 +1096,360 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add dZAP1, source data, change filenames
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/GRN_Gene_Lists.xlsx
+++ b/data/GRNmap_input_workbooks/GRN_Gene_Lists.xlsx
@@ -19,7 +19,7 @@
     <sheet name="dZAP1_gene_list" sheetId="5" r:id="rId5"/>
     <sheet name="all-strains_gene_list" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="34">
   <si>
     <t>ABF1</t>
   </si>
@@ -125,13 +125,19 @@
   </si>
   <si>
     <t>dZAP1_list</t>
+  </si>
+  <si>
+    <t>HSF1</t>
+  </si>
+  <si>
+    <t>MCM1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,11 +146,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -164,14 +169,19 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,24 +191,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -236,21 +228,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -602,96 +588,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="11" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -708,84 +703,87 @@
       <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="11" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -808,80 +806,83 @@
       <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="11" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -904,85 +905,88 @@
       <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="11" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -999,91 +1003,99 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="11" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1100,22 +1112,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D29" activeCellId="1" sqref="A29:B29 D29:E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>27</v>
       </c>
@@ -1132,319 +1144,351 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="12" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="D6" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="E8" s="1" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E11" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="12" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E18" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="12" t="s">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12" t="s">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9" t="s">
+      <c r="B24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E24" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="D25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="11"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" t="s">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9" t="s">
+      <c r="C29" s="3"/>
+      <c r="D29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E29" s="6" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corrected error in "all-strains" sheet
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/GRN_Gene_Lists.xlsx
+++ b/data/GRNmap_input_workbooks/GRN_Gene_Lists.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdahlqui\Documents\GitClone_DahlquistLab_20160622b\DahlquistLab\data\GRNmap_input_workbooks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11205" yWindow="1815" windowWidth="25605" windowHeight="13965" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="11205" yWindow="1815" windowWidth="25605" windowHeight="13965" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="wt_gene_list" sheetId="1" r:id="rId1"/>
@@ -1115,7 +1110,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" activeCellId="1" sqref="A29:B29 D29:E29"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1414,9 +1409,7 @@
       <c r="A24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
         <v>11</v>
       </c>
@@ -1429,7 +1422,9 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C25" s="3" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Added both gene lists for new CIN5 networks
Added edited one and added another column for dCIN5 network gene list. The first column for dCIN5 is for the 17 gene and 32 edges network while the second column is for the 14 gene, 25 edge network.
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/GRN_Gene_Lists.xlsx
+++ b/data/GRNmap_input_workbooks/GRN_Gene_Lists.xlsx
@@ -1,30 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="11205" yWindow="1815" windowWidth="25605" windowHeight="13965" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="wt_gene_list" sheetId="1" r:id="rId1"/>
-    <sheet name="dCIN5_gene_list" sheetId="2" r:id="rId2"/>
+    <sheet name="dCIN5_17-gene_list" sheetId="2" r:id="rId2"/>
     <sheet name="dGLN3_gene_list" sheetId="3" r:id="rId3"/>
     <sheet name="dHAP4_gene_list" sheetId="4" r:id="rId4"/>
     <sheet name="dZAP1_gene_list" sheetId="5" r:id="rId5"/>
     <sheet name="all-strains_gene_list" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="34">
   <si>
     <t>ABF1</t>
   </si>
@@ -80,9 +75,6 @@
     <t>MGA2</t>
   </si>
   <si>
-    <t>PDR1</t>
-  </si>
-  <si>
     <t>RDS3</t>
   </si>
   <si>
@@ -110,9 +102,6 @@
     <t>wt_list</t>
   </si>
   <si>
-    <t>dCIN5_list</t>
-  </si>
-  <si>
     <t>dGLN3_list</t>
   </si>
   <si>
@@ -126,15 +115,28 @@
   </si>
   <si>
     <t>MCM1</t>
+  </si>
+  <si>
+    <t>dCIN5_14-gene_list</t>
+  </si>
+  <si>
+    <t>dCIN5_17-gene_list</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -208,32 +210,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="14"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -247,15 +252,14 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="14"/>
+    <cellStyle name="Normal 3" xfId="13"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -621,7 +625,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
@@ -692,10 +696,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -709,87 +713,92 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -818,7 +827,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
@@ -848,7 +857,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
@@ -863,12 +872,12 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
@@ -917,7 +926,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
@@ -957,7 +966,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
@@ -967,7 +976,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
@@ -1031,7 +1040,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
@@ -1061,12 +1070,12 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
@@ -1081,7 +1090,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
@@ -1107,94 +1116,103 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="3" max="3" width="8.625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="9.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C6" s="3"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1210,37 +1228,43 @@
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>16</v>
@@ -1254,8 +1278,11 @@
       <c r="E11" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
@@ -1271,8 +1298,11 @@
       <c r="E12" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>7</v>
       </c>
@@ -1288,12 +1318,17 @@
       <c r="E13" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="C14" s="6" t="s">
         <v>8</v>
       </c>
@@ -1303,37 +1338,47 @@
       <c r="E14" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
@@ -1349,37 +1394,43 @@
       <c r="E18" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
@@ -1392,24 +1443,32 @@
       <c r="D22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C24" s="3" t="s">
         <v>11</v>
       </c>
@@ -1419,30 +1478,37 @@
       <c r="E24" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>12</v>
       </c>
@@ -1455,9 +1521,12 @@
       <c r="D27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>13</v>
       </c>
@@ -1470,20 +1539,24 @@
       <c r="D28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="6" t="s">
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="F29" s="6" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rename networks db1, db2, etc.
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/GRN_Gene_Lists.xlsx
+++ b/data/GRNmap_input_workbooks/GRN_Gene_Lists.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdahlqui\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11205" yWindow="1815" windowWidth="25605" windowHeight="13965" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="11205" yWindow="1815" windowWidth="25605" windowHeight="13965" tabRatio="695" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="wt_gene_list" sheetId="1" r:id="rId1"/>
-    <sheet name="dCIN5_17-gene_list" sheetId="2" r:id="rId2"/>
-    <sheet name="dGLN3_gene_list" sheetId="3" r:id="rId3"/>
-    <sheet name="dHAP4_gene_list" sheetId="4" r:id="rId4"/>
-    <sheet name="dZAP1_gene_list" sheetId="5" r:id="rId5"/>
-    <sheet name="all-strains_gene_list" sheetId="6" r:id="rId6"/>
+    <sheet name="db1_wt_gene_list" sheetId="1" r:id="rId1"/>
+    <sheet name="db3_dCIN5_17-gene_list" sheetId="2" r:id="rId2"/>
+    <sheet name="db4_dGLN3_gene_list" sheetId="3" r:id="rId3"/>
+    <sheet name="db5_dHAP4_gene_list" sheetId="4" r:id="rId4"/>
+    <sheet name="db6_dZAP1_gene_list" sheetId="5" r:id="rId5"/>
+    <sheet name="all_networks_gene_list" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000"/>
 </workbook>
@@ -99,44 +104,50 @@
     <t>CST6</t>
   </si>
   <si>
-    <t>wt_list</t>
-  </si>
-  <si>
-    <t>dGLN3_list</t>
-  </si>
-  <si>
-    <t>dHAP4_list</t>
-  </si>
-  <si>
-    <t>dZAP1_list</t>
-  </si>
-  <si>
     <t>HSF1</t>
   </si>
   <si>
     <t>MCM1</t>
   </si>
   <si>
-    <t>dCIN5_14-gene_list</t>
-  </si>
-  <si>
-    <t>dCIN5_17-gene_list</t>
-  </si>
-  <si>
     <t>all_genes</t>
+  </si>
+  <si>
+    <t>db1</t>
+  </si>
+  <si>
+    <t>db2</t>
+  </si>
+  <si>
+    <t>db3</t>
+  </si>
+  <si>
+    <t>db4</t>
+  </si>
+  <si>
+    <t>db5</t>
+  </si>
+  <si>
+    <t>db6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -181,7 +192,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +202,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,31 +232,34 @@
   </borders>
   <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="14"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="14"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -263,6 +283,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -716,87 +739,87 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>31</v>
+      <c r="A8" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1073,12 +1096,12 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
@@ -1121,521 +1144,519 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="9.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="1" max="2" width="5.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="G15" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="H4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="H9" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="G17" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="G18" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3" t="s">
+    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3" t="s">
+      <c r="E19" s="8"/>
+      <c r="F19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="G19" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="H20" s="3" t="s">
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="H21" s="3" t="s">
+      <c r="F21" s="8"/>
+      <c r="G21" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3" t="s">
+    <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3" t="s">
+      <c r="D22" s="8"/>
+      <c r="E22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="H22" s="3" t="s">
+      <c r="F22" s="8"/>
+      <c r="G22" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="G23" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3" t="s">
+    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="3"/>
-      <c r="H24" s="3" t="s">
+      <c r="F24" s="8"/>
+      <c r="G24" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
+    <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="H25" s="3" t="s">
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="H26" s="3" t="s">
+      <c r="F26" s="8"/>
+      <c r="G26" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="3"/>
-      <c r="H27" s="3" t="s">
+      <c r="F27" s="8"/>
+      <c r="G27" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6" t="s">
+      <c r="D28" s="9"/>
+      <c r="E28" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="G28" s="9" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>